<commit_message>
New features on reactable and wip to collect data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avanstraaten/21Goals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9C1190-AE67-4F45-B950-E69989BE37A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8953CA3A-2AF4-064A-BC5A-DDC2E087A664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{8E9E23B5-BE8D-1F40-92DE-C041C0BDFAFD}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +119,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,14 +149,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,7 +495,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,7 +675,7 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -724,6 +735,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{A042C5D3-1111-8841-A4CF-0B2E5D328950}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add functions to collect players informations
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avanstraaten/21Goals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD523E11-FAF5-EF4C-8801-A1856C9E7DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F1C42-C5DA-9B4B-9950-C6A192854EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{8E9E23B5-BE8D-1F40-92DE-C041C0BDFAFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>player</t>
   </si>
@@ -53,31 +53,124 @@
     <t>Kvaradona</t>
   </si>
   <si>
-    <t>Fan de Kroupie</t>
-  </si>
-  <si>
-    <t>Mbappe Lover</t>
-  </si>
-  <si>
-    <t>RCK</t>
-  </si>
-  <si>
-    <t>Tokpa FC</t>
-  </si>
-  <si>
-    <t>Ludovic Blas</t>
-  </si>
-  <si>
-    <t>Adrien Tuffert</t>
-  </si>
-  <si>
-    <t>Arnaud Kalimuendo</t>
-  </si>
-  <si>
     <t>Hakimi</t>
   </si>
   <si>
     <t>Vitinha</t>
+  </si>
+  <si>
+    <t>Hakimi (AOAT (Africain Of All Time))</t>
+  </si>
+  <si>
+    <t>Joao Neves (le GOAT)</t>
+  </si>
+  <si>
+    <t>Tosin (Béninois sauvage)</t>
+  </si>
+  <si>
+    <t>Sambou Soumano (le magicien Sénégalais)</t>
+  </si>
+  <si>
+    <t>Golovin</t>
+  </si>
+  <si>
+    <t>Pogba</t>
+  </si>
+  <si>
+    <t>Tolisso</t>
+  </si>
+  <si>
+    <t>Tagliafio</t>
+  </si>
+  <si>
+    <t>Djaoui Cissé</t>
+  </si>
+  <si>
+    <t>Moses Simon</t>
+  </si>
+  <si>
+    <t>Clauss</t>
+  </si>
+  <si>
+    <t>Gboho</t>
+  </si>
+  <si>
+    <t>Rongier</t>
+  </si>
+  <si>
+    <t>Nuno</t>
+  </si>
+  <si>
+    <t>Haraldson</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>Gwen</t>
+  </si>
+  <si>
+    <t>Alain</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/e42d61c7/Achraf-Hakimi</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/c0c7ff58/Fabian-Ruiz-Pena</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/dea88efd/Khvicha-Kvaratskhelia</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/3b029691/Vitinha</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/c2a15a27/Joao-Neves</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/9c4f39b3/Tosin-Aiyegun</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/7cc00776/Sambou-Soumano</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/3708e9fa/Aleksandr-Golovin</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/867239d3/Paul-Pogba</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/652d4c37/Corentin-Tolisso</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/f0661424/Nicolas-Tagliafico</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/576ca93f/Djaoui-Cisse</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/5f3eaaf5/Moses-Simon</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/5219ab4a/Jonathan-Clauss</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/6be41a31/Yann-Gboho</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/ed45c4a5/Valentin-Rongier</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/f20e4cc9/Nuno-Mendes</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/e2ae54db/Hakon-Arnar-Haraldsson</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
@@ -449,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3044FC0B-61DE-9448-9E0E-B8EB7C0F96D6}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,172 +553,235 @@
     <col min="1" max="1" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New features with others stats & background-image
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avanstraaten/21Goals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F1C42-C5DA-9B4B-9950-C6A192854EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2555D2B2-6031-0B42-8FCC-28D0D5A447D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{8E9E23B5-BE8D-1F40-92DE-C041C0BDFAFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
   <si>
     <t>player</t>
   </si>
@@ -171,16 +171,53 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>Emilie</t>
+  </si>
+  <si>
+    <t>Ludovic Blas</t>
+  </si>
+  <si>
+    <t>Marquinhos</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/d5f2f82b/Marquinhos</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/6191093d/Ludovic-Blas</t>
+  </si>
+  <si>
+    <t>Léna</t>
+  </si>
+  <si>
+    <t>Maupay</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/76a82373/Carlos-Gomez</t>
+  </si>
+  <si>
+    <t>Carlos Gomez</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/4bcf39f6/Neal-Maupay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,8 +243,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,15 +580,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3044FC0B-61DE-9448-9E0E-B8EB7C0F96D6}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -784,6 +823,94 @@
         <v>43</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new player & WIP on cumulative chart
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avanstraaten/21Goals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2555D2B2-6031-0B42-8FCC-28D0D5A447D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D1D017-17DB-B841-AFD0-687AFFF22413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{8E9E23B5-BE8D-1F40-92DE-C041C0BDFAFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>player</t>
   </si>
@@ -201,6 +201,33 @@
   </si>
   <si>
     <t>https://fbref.com/en/players/4bcf39f6/Neal-Maupay</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Pagis</t>
+  </si>
+  <si>
+    <t>Egan Riley</t>
+  </si>
+  <si>
+    <t>Tessman</t>
+  </si>
+  <si>
+    <t>Kechta</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/7d827b4f/Pablo-Pagis</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/d313e8ff/CJ-Egan-Riley</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/ac277993/Tanner-Tessmann</t>
+  </si>
+  <si>
+    <t>https://fbref.com/en/players/abefc3af/Yassine-Kechta</t>
   </si>
 </sst>
 </file>
@@ -580,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3044FC0B-61DE-9448-9E0E-B8EB7C0F96D6}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -911,6 +938,50 @@
         <v>52</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>